<commit_message>
Update for part 2
</commit_message>
<xml_diff>
--- a/Assignment_1/Problem_2/CNN_NB_parameters.xlsx
+++ b/Assignment_1/Problem_2/CNN_NB_parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usele\Documents\Cours\IFT6135\TP1\IFT6135-H2019-Programming\Assignment_1\Problem_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{020CC381-420B-4D1F-BEEB-103AC3F4A72F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81ADE88B-ADA8-4ABC-90A6-AA25FE9AEF2D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24669" windowHeight="9283" xr2:uid="{CCDCEB27-87F1-405A-AD12-B82BEBDA3D72}"/>
   </bookViews>
@@ -147,10 +147,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47ACEF9D-ECF7-425A-8A27-09021956ABED}">
-  <dimension ref="A1:P38"/>
+  <dimension ref="A1:P37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -486,25 +489,25 @@
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="3" t="s">
         <v>24</v>
       </c>
     </row>
@@ -584,11 +587,11 @@
       <c r="B5" s="1"/>
       <c r="C5" s="1">
         <f>(C4-F5+2*H5)/G5+1</f>
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D5" s="1">
         <f>(D4-F5+2*H5)/G5+1</f>
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E5" s="1">
         <v>32</v>
@@ -600,10 +603,10 @@
         <v>1</v>
       </c>
       <c r="H5" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I5" s="1">
-        <f>E5*B4</f>
+        <f>E5</f>
         <v>32</v>
       </c>
       <c r="J5" s="1">
@@ -627,7 +630,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="2">
         <f>C5/B6</f>
@@ -739,14 +742,14 @@
       </c>
       <c r="C13" s="1">
         <f>(C12-F13+2*H13)/G13+1</f>
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D13" s="1">
         <f>(D12-F13+2*H13)/G13+1</f>
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E13" s="1">
-        <v>32</v>
+        <v>87</v>
       </c>
       <c r="F13" s="1">
         <v>3</v>
@@ -755,15 +758,15 @@
         <v>1</v>
       </c>
       <c r="H13" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I13" s="1">
-        <f>E13*B12</f>
-        <v>32</v>
+        <f>E13</f>
+        <v>87</v>
       </c>
       <c r="J13" s="1">
         <f>(F13*F13*B12+1)*E13</f>
-        <v>320</v>
+        <v>870</v>
       </c>
       <c r="L13" s="1">
         <f>M12+1</f>
@@ -782,15 +785,15 @@
         <v>11</v>
       </c>
       <c r="B14" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C14" s="2">
         <f>C13/B14</f>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D14" s="2">
         <f>D13/B14</f>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -805,18 +808,18 @@
       </c>
       <c r="B15" s="1">
         <f>I13</f>
-        <v>32</v>
+        <v>87</v>
       </c>
       <c r="C15" s="1">
         <f>(C14-F15+2*H15)/G15+1</f>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D15" s="1">
         <f>(D14-F15+2*H15)/G15+1</f>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E15" s="1">
-        <v>16</v>
+        <v>512</v>
       </c>
       <c r="F15" s="1">
         <v>3</v>
@@ -828,12 +831,12 @@
         <v>1</v>
       </c>
       <c r="I15" s="1">
-        <f>E15*B15</f>
+        <f>E15</f>
         <v>512</v>
       </c>
       <c r="J15" s="1">
         <f>(F15*F15*I13+1)*I15</f>
-        <v>147968</v>
+        <v>401408</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.4">
@@ -841,7 +844,7 @@
         <v>11</v>
       </c>
       <c r="B16" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C16" s="2">
         <f>C15/B16</f>
@@ -862,7 +865,7 @@
       </c>
       <c r="N16" s="1">
         <f>N13+N12+J15+J13</f>
-        <v>549962</v>
+        <v>803952</v>
       </c>
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
@@ -960,14 +963,14 @@
       </c>
       <c r="C22" s="1">
         <f>(C21-F22+2*H22)/G22+1</f>
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D22" s="1">
         <f>(D21-F22+2*H22)/G22+1</f>
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E22" s="1">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="F22" s="1">
         <v>3</v>
@@ -976,15 +979,15 @@
         <v>1</v>
       </c>
       <c r="H22" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I22" s="1">
-        <f>E22*B21</f>
-        <v>32</v>
+        <f>E22</f>
+        <v>64</v>
       </c>
       <c r="J22" s="1">
         <f>(F22*F22*B21+1)*E22</f>
-        <v>320</v>
+        <v>640</v>
       </c>
       <c r="K22" s="1"/>
       <c r="L22" s="1">
@@ -1005,15 +1008,15 @@
         <v>11</v>
       </c>
       <c r="B23" s="1">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C23" s="2">
         <f>C22/B23</f>
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D23" s="2">
         <f>D22/B23</f>
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
@@ -1033,18 +1036,18 @@
       </c>
       <c r="B24" s="1">
         <f>I22</f>
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="C24" s="1">
         <f>(C23-F24+2*H24)/G24+1</f>
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D24" s="1">
         <f>(D23-F24+2*H24)/G24+1</f>
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="E24" s="1">
-        <v>2</v>
+        <v>77</v>
       </c>
       <c r="F24" s="1">
         <v>3</v>
@@ -1056,12 +1059,12 @@
         <v>1</v>
       </c>
       <c r="I24" s="1">
-        <f>E24*B24</f>
-        <v>64</v>
+        <f>E24</f>
+        <v>77</v>
       </c>
       <c r="J24" s="1">
         <f>(F24*F24*I22+1)*I24</f>
-        <v>18496</v>
+        <v>44429</v>
       </c>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
@@ -1078,11 +1081,11 @@
       </c>
       <c r="C25" s="2">
         <f>C24/B25</f>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D25" s="2">
         <f>D24/B25</f>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
@@ -1102,18 +1105,18 @@
       </c>
       <c r="B26" s="1">
         <f>I24</f>
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="C26" s="1">
         <f>(C25-F26+2*H26)/G26+1</f>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D26" s="1">
         <f>(D25-F26+2*H26)/G26+1</f>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E26" s="1">
-        <v>8</v>
+        <v>512</v>
       </c>
       <c r="F26" s="1">
         <v>3</v>
@@ -1125,12 +1128,12 @@
         <v>1</v>
       </c>
       <c r="I26" s="1">
-        <f>E26*B26</f>
+        <f>E26</f>
         <v>512</v>
       </c>
       <c r="J26" s="1">
         <f>(F26*F26*I24+1)*I26</f>
-        <v>295424</v>
+        <v>355328</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.4">
@@ -1138,7 +1141,7 @@
         <v>11</v>
       </c>
       <c r="B27">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C27">
         <f>C26/B27</f>
@@ -1153,7 +1156,7 @@
       </c>
       <c r="N27" s="1">
         <f>N22+J24+N21+J26+J22</f>
-        <v>715914</v>
+        <v>802071</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.4">
@@ -1242,15 +1245,9 @@
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
     </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.4">
-      <c r="N38" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="C14:D14" formula="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
 

</xml_diff>